<commit_message>
new management scenarios test
</commit_message>
<xml_diff>
--- a/Models/Inputs/management_scenarios/new scenarios 2022-09-19.xlsx
+++ b/Models/Inputs/management_scenarios/new scenarios 2022-09-19.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\Research\TCSI conservation finance\Models\Inputs\management_scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD95FF3-25D0-41CC-AF95-F3FC854B89BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F57E0AB-15FC-492B-87BC-94D7C59C70B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="1140" windowWidth="18000" windowHeight="9360" xr2:uid="{3EDC2C11-82F6-48B8-9EB3-22FBBA12C335}"/>
+    <workbookView xWindow="540" yWindow="2730" windowWidth="15360" windowHeight="9360" xr2:uid="{3EDC2C11-82F6-48B8-9EB3-22FBBA12C335}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,7 @@
   <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,13 +457,13 @@
         <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -474,13 +474,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -491,13 +491,13 @@
         <v>6</v>
       </c>
       <c r="C4" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -508,13 +508,13 @@
         <v>7</v>
       </c>
       <c r="C5" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -525,13 +525,13 @@
         <v>8</v>
       </c>
       <c r="C6" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="E8">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -576,13 +576,13 @@
         <v>9</v>
       </c>
       <c r="C9" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -593,13 +593,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -610,13 +610,13 @@
         <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,13 +627,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -644,13 +644,13 @@
         <v>8</v>
       </c>
       <c r="C13" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -661,13 +661,13 @@
         <v>9</v>
       </c>
       <c r="C14" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -678,13 +678,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -695,13 +695,13 @@
         <v>6</v>
       </c>
       <c r="C16" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -712,13 +712,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -729,13 +729,13 @@
         <v>8</v>
       </c>
       <c r="C18" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
         <v>0</v>
       </c>
       <c r="E19">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>0</v>
       </c>
       <c r="E20">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -786,7 +786,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -797,13 +797,13 @@
         <v>5</v>
       </c>
       <c r="C22" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -814,13 +814,13 @@
         <v>6</v>
       </c>
       <c r="C23" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -831,13 +831,13 @@
         <v>7</v>
       </c>
       <c r="C24" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -848,13 +848,13 @@
         <v>8</v>
       </c>
       <c r="C25" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -865,13 +865,13 @@
         <v>9</v>
       </c>
       <c r="C26" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -882,13 +882,13 @@
         <v>5</v>
       </c>
       <c r="C27" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -899,13 +899,13 @@
         <v>6</v>
       </c>
       <c r="C28" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -916,13 +916,13 @@
         <v>7</v>
       </c>
       <c r="C29" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -933,13 +933,13 @@
         <v>8</v>
       </c>
       <c r="C30" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -956,7 +956,7 @@
         <v>0</v>
       </c>
       <c r="E31">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -973,7 +973,7 @@
         <v>0</v>
       </c>
       <c r="E32">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -990,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1001,13 +1001,13 @@
         <v>5</v>
       </c>
       <c r="C34" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,13 +1018,13 @@
         <v>6</v>
       </c>
       <c r="C35" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1035,13 +1035,13 @@
         <v>7</v>
       </c>
       <c r="C36" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1052,13 +1052,13 @@
         <v>8</v>
       </c>
       <c r="C37" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1069,13 +1069,13 @@
         <v>9</v>
       </c>
       <c r="C38" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1086,13 +1086,13 @@
         <v>5</v>
       </c>
       <c r="C39" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1103,13 +1103,13 @@
         <v>6</v>
       </c>
       <c r="C40" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1120,13 +1120,13 @@
         <v>7</v>
       </c>
       <c r="C41" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,13 +1137,13 @@
         <v>8</v>
       </c>
       <c r="C42" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1160,7 +1160,7 @@
         <v>0</v>
       </c>
       <c r="E43">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1177,7 +1177,7 @@
         <v>0</v>
       </c>
       <c r="E44">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1188,13 +1188,13 @@
         <v>5</v>
       </c>
       <c r="C45" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1205,13 +1205,13 @@
         <v>6</v>
       </c>
       <c r="C46" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1222,13 +1222,13 @@
         <v>7</v>
       </c>
       <c r="C47" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1239,13 +1239,13 @@
         <v>8</v>
       </c>
       <c r="C48" s="1">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1256,13 +1256,13 @@
         <v>9</v>
       </c>
       <c r="C49" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1273,13 +1273,13 @@
         <v>5</v>
       </c>
       <c r="C50" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1290,13 +1290,13 @@
         <v>6</v>
       </c>
       <c r="C51" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1307,13 +1307,13 @@
         <v>7</v>
       </c>
       <c r="C52" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1324,13 +1324,13 @@
         <v>8</v>
       </c>
       <c r="C53" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1341,13 +1341,13 @@
         <v>6</v>
       </c>
       <c r="C54" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,13 +1358,13 @@
         <v>7</v>
       </c>
       <c r="C55" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>